<commit_message>
fix: Dates error, SQL Arrays error, Not updated files error, not updated Global rating error...
</commit_message>
<xml_diff>
--- a/Resources/Sources/Template_Competition.xlsx
+++ b/Resources/Sources/Template_Competition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Igor\Programming\Femida_v3\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Igor\Programming\Femida_v3\Resources\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5BA43A-BE82-44A7-8A29-15DBA3A319ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08FC049-71D7-494E-B233-3B0675208B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заполнение" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Название соревнования:</t>
   </si>
@@ -146,136 +146,10 @@
     <t>Существующие судьи</t>
   </si>
   <si>
-    <t>Саяфаров</t>
-  </si>
-  <si>
-    <t>Валерий</t>
-  </si>
-  <si>
-    <t>Сабирьянович</t>
-  </si>
-  <si>
-    <t>Саяфаров Валерий Сабирьянович</t>
-  </si>
-  <si>
-    <t>Ершов</t>
-  </si>
-  <si>
-    <t>Александр</t>
-  </si>
-  <si>
-    <t>Валентинович</t>
-  </si>
-  <si>
-    <t>Ершов Александр Валентинович</t>
-  </si>
-  <si>
-    <t>Марченко</t>
-  </si>
-  <si>
-    <t>Юрий</t>
-  </si>
-  <si>
-    <t>Анатольевич</t>
-  </si>
-  <si>
-    <t>Марченко Юрий Анатольевич</t>
-  </si>
-  <si>
-    <t>Соловьев</t>
-  </si>
-  <si>
-    <t>Вячеславович</t>
-  </si>
-  <si>
-    <t>Соловьев Александр Вячеславович</t>
-  </si>
-  <si>
-    <t>Панаков</t>
-  </si>
-  <si>
-    <t>Дивлохович</t>
-  </si>
-  <si>
-    <t>Панаков Александр Дивлохович</t>
-  </si>
-  <si>
-    <t>Ушаков</t>
-  </si>
-  <si>
-    <t>Евгеньевич</t>
-  </si>
-  <si>
-    <t>Ушаков Александр Евгеньевич</t>
-  </si>
-  <si>
-    <t>Духов</t>
-  </si>
-  <si>
-    <t>Михаил</t>
-  </si>
-  <si>
-    <t>Валерьевич</t>
-  </si>
-  <si>
-    <t>Духов Михаил Валерьевич</t>
-  </si>
-  <si>
-    <t>Алексанов</t>
-  </si>
-  <si>
-    <t>Андрей</t>
-  </si>
-  <si>
-    <t>Николаевич</t>
-  </si>
-  <si>
-    <t>Алексанов Андрей Николаевич</t>
-  </si>
-  <si>
-    <t>Пролубников</t>
-  </si>
-  <si>
-    <t>Олег</t>
-  </si>
-  <si>
-    <t>Пролубников Олег Николаевич</t>
-  </si>
-  <si>
-    <t>Битук</t>
-  </si>
-  <si>
-    <t>Евгений</t>
-  </si>
-  <si>
-    <t>Иванович</t>
-  </si>
-  <si>
-    <t>Битук Евгений Иванович</t>
-  </si>
-  <si>
     <t>ФИО</t>
   </si>
   <si>
     <t>Секундометрист</t>
-  </si>
-  <si>
-    <t>Первый</t>
-  </si>
-  <si>
-    <t>1 и 2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Москва</t>
-  </si>
-  <si>
-    <t>Супер соревнование</t>
   </si>
 </sst>
 </file>
@@ -1281,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,9 +1234,7 @@
       <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="50" t="s">
-        <v>70</v>
-      </c>
+      <c r="D7" s="50"/>
       <c r="E7" s="51"/>
       <c r="F7" s="52"/>
       <c r="U7" s="2" t="s">
@@ -1374,9 +1246,7 @@
       <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="50" t="s">
-        <v>69</v>
-      </c>
+      <c r="D8" s="50"/>
       <c r="E8" s="51"/>
       <c r="F8" s="52"/>
       <c r="U8" s="2" t="s">
@@ -1388,13 +1258,11 @@
       <c r="C9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="53">
-        <v>45006</v>
-      </c>
+      <c r="D9" s="53"/>
       <c r="E9" s="54"/>
       <c r="F9" s="55"/>
       <c r="U9" s="2" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -1423,7 +1291,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>10</v>
@@ -1439,73 +1307,41 @@
       <c r="B13" s="6">
         <v>1</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="36">
-        <v>10</v>
-      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
+      <c r="B14" s="6" t="str">
         <f>IF(C14="","",B13+1)</f>
-        <v>2</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="36">
-        <v>10</v>
-      </c>
+        <v/>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
+      <c r="B15" s="6" t="str">
         <f t="shared" ref="B15:B78" si="0">IF(C15="","",B14+1)</f>
-        <v>3</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="36">
-        <v>10</v>
-      </c>
+        <v/>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="36"/>
       <c r="H15" s="45"/>
     </row>
     <row r="16" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="36">
-        <v>9</v>
-      </c>
+      <c r="B16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="str">
@@ -2506,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FFBD96-15EE-4547-B7E4-6358D9EC97D9}">
-  <dimension ref="B2:E13"/>
+  <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2519,14 +2355,14 @@
     <col min="5" max="16384" width="9.140625" style="47"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="56" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="56"/>
       <c r="D2" s="56"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="46" t="s">
         <v>4</v>
       </c>
@@ -2535,146 +2371,6 @@
       </c>
       <c r="D3" s="46" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="47" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="47" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="47" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="47" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="47" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="47" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="47" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="47" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2840,7 +2536,7 @@
       </c>
       <c r="B11" s="24" t="str">
         <f>IF(Заполнение!C13="","",Заполнение!C13)</f>
-        <v>Саяфаров Валерий Сабирьянович</v>
+        <v/>
       </c>
       <c r="C11" s="69" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
@@ -2853,11 +2549,11 @@
       </c>
       <c r="F11" s="25" t="str">
         <f>IF(Заполнение!D13="","",Заполнение!D13)</f>
-        <v>Главный судья соревнований</v>
-      </c>
-      <c r="G11" s="23">
+        <v/>
+      </c>
+      <c r="G11" s="23" t="str">
         <f>IF(Заполнение!F13="","",Заполнение!F13)</f>
-        <v>10</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2867,7 +2563,7 @@
       </c>
       <c r="B12" s="24" t="str">
         <f>IF(Заполнение!C14="","",Заполнение!C14)</f>
-        <v>Панаков Александр Дивлохович</v>
+        <v/>
       </c>
       <c r="C12" s="59" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
@@ -2880,11 +2576,11 @@
       </c>
       <c r="F12" s="26" t="str">
         <f>IF(Заполнение!D14="","",Заполнение!D14)</f>
-        <v>Рефери</v>
-      </c>
-      <c r="G12" s="23">
+        <v/>
+      </c>
+      <c r="G12" s="23" t="str">
         <f>IF(Заполнение!F14="","",Заполнение!F14)</f>
-        <v>10</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2894,7 +2590,7 @@
       </c>
       <c r="B13" s="24" t="str">
         <f>IF(Заполнение!C15="","",Заполнение!C15)</f>
-        <v>Ушаков Александр Евгеньевич</v>
+        <v/>
       </c>
       <c r="C13" s="59" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
@@ -2907,11 +2603,11 @@
       </c>
       <c r="F13" s="26" t="str">
         <f>IF(Заполнение!D15="","",Заполнение!D15)</f>
-        <v>Боковой судья</v>
-      </c>
-      <c r="G13" s="23">
+        <v/>
+      </c>
+      <c r="G13" s="23" t="str">
         <f>IF(Заполнение!F15="","",Заполнение!F15)</f>
-        <v>10</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2921,7 +2617,7 @@
       </c>
       <c r="B14" s="24" t="str">
         <f>IF(Заполнение!C16="","",Заполнение!C16)</f>
-        <v>Ершов Александр Валентинович</v>
+        <v/>
       </c>
       <c r="C14" s="59" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
@@ -2934,11 +2630,11 @@
       </c>
       <c r="F14" s="26" t="str">
         <f>IF(Заполнение!D16="","",Заполнение!D16)</f>
-        <v>Секундометрист</v>
-      </c>
-      <c r="G14" s="23">
+        <v/>
+      </c>
+      <c r="G14" s="23" t="str">
         <f>IF(Заполнение!F16="","",Заполнение!F16)</f>
-        <v>9</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3898,7 +3594,7 @@
       <c r="E53" s="65"/>
       <c r="F53" s="66" t="str">
         <f ca="1">"Дата: " &amp; TEXT(TODAY(),"ДД.ММ.ГГГГ")</f>
-        <v>Дата: 21.03.2023</v>
+        <v>Дата: 23.03.2023</v>
       </c>
       <c r="G53" s="66"/>
       <c r="I53" s="35"/>

</xml_diff>

<commit_message>
feat: Roles; JAR build fixes
</commit_message>
<xml_diff>
--- a/Resources/Sources/Template_Competition.xlsx
+++ b/Resources/Sources/Template_Competition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Igor\Programming\Femida_v3\Resources\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08FC049-71D7-494E-B233-3B0675208B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC684532-329F-4135-9876-C6C116C854B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24915" yWindow="3840" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заполнение" sheetId="1" r:id="rId1"/>
@@ -742,22 +742,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -768,6 +752,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -779,6 +769,16 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1155,9 +1155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X111"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2344,7 +2342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FFBD96-15EE-4547-B7E4-6358D9EC97D9}">
   <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -2405,37 +2403,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
       <c r="H1" s="11"/>
       <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
       <c r="H2" s="11"/>
       <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="11"/>
       <c r="I3" s="12"/>
     </row>
@@ -2479,11 +2477,11 @@
       <c r="C7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="64" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E7" s="64"/>
+      <c r="D7" s="58" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E7" s="58"/>
       <c r="F7" s="14"/>
       <c r="G7" s="16"/>
     </row>
@@ -2493,10 +2491,10 @@
       <c r="C8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="63">
+      <c r="D8" s="57">
         <v>1</v>
       </c>
-      <c r="E8" s="63"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="14"/>
       <c r="G8" s="16"/>
     </row>
@@ -2516,10 +2514,10 @@
       <c r="B10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="67" t="s">
+      <c r="C10" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="68"/>
+      <c r="D10" s="64"/>
       <c r="E10" s="21" t="s">
         <v>6</v>
       </c>
@@ -2538,11 +2536,11 @@
         <f>IF(Заполнение!C13="","",Заполнение!C13)</f>
         <v/>
       </c>
-      <c r="C11" s="69" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D11" s="70"/>
+      <c r="C11" s="65" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D11" s="66"/>
       <c r="E11" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2565,11 +2563,11 @@
         <f>IF(Заполнение!C14="","",Заполнение!C14)</f>
         <v/>
       </c>
-      <c r="C12" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D12" s="60"/>
+      <c r="C12" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D12" s="62"/>
       <c r="E12" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2592,11 +2590,11 @@
         <f>IF(Заполнение!C15="","",Заполнение!C15)</f>
         <v/>
       </c>
-      <c r="C13" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D13" s="60"/>
+      <c r="C13" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D13" s="62"/>
       <c r="E13" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2619,11 +2617,11 @@
         <f>IF(Заполнение!C16="","",Заполнение!C16)</f>
         <v/>
       </c>
-      <c r="C14" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D14" s="60"/>
+      <c r="C14" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D14" s="62"/>
       <c r="E14" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2646,11 +2644,11 @@
         <f>IF(Заполнение!C17="","",Заполнение!C17)</f>
         <v/>
       </c>
-      <c r="C15" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D15" s="60"/>
+      <c r="C15" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D15" s="62"/>
       <c r="E15" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2673,11 +2671,11 @@
         <f>IF(Заполнение!C18="","",Заполнение!C18)</f>
         <v/>
       </c>
-      <c r="C16" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D16" s="60"/>
+      <c r="C16" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D16" s="62"/>
       <c r="E16" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2700,11 +2698,11 @@
         <f>IF(Заполнение!C19="","",Заполнение!C19)</f>
         <v/>
       </c>
-      <c r="C17" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D17" s="60"/>
+      <c r="C17" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D17" s="62"/>
       <c r="E17" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2727,11 +2725,11 @@
         <f>IF(Заполнение!C20="","",Заполнение!C20)</f>
         <v/>
       </c>
-      <c r="C18" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D18" s="60"/>
+      <c r="C18" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D18" s="62"/>
       <c r="E18" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2754,11 +2752,11 @@
         <f>IF(Заполнение!C21="","",Заполнение!C21)</f>
         <v/>
       </c>
-      <c r="C19" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D19" s="60"/>
+      <c r="C19" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D19" s="62"/>
       <c r="E19" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2781,11 +2779,11 @@
         <f>IF(Заполнение!C22="","",Заполнение!C22)</f>
         <v/>
       </c>
-      <c r="C20" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D20" s="60"/>
+      <c r="C20" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D20" s="62"/>
       <c r="E20" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2808,11 +2806,11 @@
         <f>IF(Заполнение!C23="","",Заполнение!C23)</f>
         <v/>
       </c>
-      <c r="C21" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D21" s="60"/>
+      <c r="C21" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D21" s="62"/>
       <c r="E21" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2835,11 +2833,11 @@
         <f>IF(Заполнение!C24="","",Заполнение!C24)</f>
         <v/>
       </c>
-      <c r="C22" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D22" s="60"/>
+      <c r="C22" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D22" s="62"/>
       <c r="E22" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2862,11 +2860,11 @@
         <f>IF(Заполнение!C25="","",Заполнение!C25)</f>
         <v/>
       </c>
-      <c r="C23" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D23" s="60"/>
+      <c r="C23" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D23" s="62"/>
       <c r="E23" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2889,11 +2887,11 @@
         <f>IF(Заполнение!C26="","",Заполнение!C26)</f>
         <v/>
       </c>
-      <c r="C24" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D24" s="60"/>
+      <c r="C24" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D24" s="62"/>
       <c r="E24" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2916,11 +2914,11 @@
         <f>IF(Заполнение!C27="","",Заполнение!C27)</f>
         <v/>
       </c>
-      <c r="C25" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D25" s="60"/>
+      <c r="C25" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D25" s="62"/>
       <c r="E25" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2943,11 +2941,11 @@
         <f>IF(Заполнение!C28="","",Заполнение!C28)</f>
         <v/>
       </c>
-      <c r="C26" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D26" s="60"/>
+      <c r="C26" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D26" s="62"/>
       <c r="E26" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2970,11 +2968,11 @@
         <f>IF(Заполнение!C29="","",Заполнение!C29)</f>
         <v/>
       </c>
-      <c r="C27" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D27" s="60"/>
+      <c r="C27" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D27" s="62"/>
       <c r="E27" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -2997,11 +2995,11 @@
         <f>IF(Заполнение!C30="","",Заполнение!C30)</f>
         <v/>
       </c>
-      <c r="C28" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D28" s="60"/>
+      <c r="C28" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D28" s="62"/>
       <c r="E28" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3024,11 +3022,11 @@
         <f>IF(Заполнение!C31="","",Заполнение!C31)</f>
         <v/>
       </c>
-      <c r="C29" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D29" s="60"/>
+      <c r="C29" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D29" s="62"/>
       <c r="E29" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3051,11 +3049,11 @@
         <f>IF(Заполнение!C32="","",Заполнение!C32)</f>
         <v/>
       </c>
-      <c r="C30" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D30" s="60"/>
+      <c r="C30" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D30" s="62"/>
       <c r="E30" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3078,11 +3076,11 @@
         <f>IF(Заполнение!C33="","",Заполнение!C33)</f>
         <v/>
       </c>
-      <c r="C31" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D31" s="60"/>
+      <c r="C31" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D31" s="62"/>
       <c r="E31" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3105,11 +3103,11 @@
         <f>IF(Заполнение!C34="","",Заполнение!C34)</f>
         <v/>
       </c>
-      <c r="C32" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D32" s="60"/>
+      <c r="C32" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D32" s="62"/>
       <c r="E32" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3132,11 +3130,11 @@
         <f>IF(Заполнение!C35="","",Заполнение!C35)</f>
         <v/>
       </c>
-      <c r="C33" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D33" s="60"/>
+      <c r="C33" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D33" s="62"/>
       <c r="E33" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3159,11 +3157,11 @@
         <f>IF(Заполнение!C36="","",Заполнение!C36)</f>
         <v/>
       </c>
-      <c r="C34" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D34" s="60"/>
+      <c r="C34" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D34" s="62"/>
       <c r="E34" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3186,11 +3184,11 @@
         <f>IF(Заполнение!C37="","",Заполнение!C37)</f>
         <v/>
       </c>
-      <c r="C35" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D35" s="60"/>
+      <c r="C35" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D35" s="62"/>
       <c r="E35" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3213,11 +3211,11 @@
         <f>IF(Заполнение!C38="","",Заполнение!C38)</f>
         <v/>
       </c>
-      <c r="C36" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D36" s="60"/>
+      <c r="C36" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D36" s="62"/>
       <c r="E36" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3240,11 +3238,11 @@
         <f>IF(Заполнение!C39="","",Заполнение!C39)</f>
         <v/>
       </c>
-      <c r="C37" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D37" s="60"/>
+      <c r="C37" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D37" s="62"/>
       <c r="E37" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3267,11 +3265,11 @@
         <f>IF(Заполнение!C40="","",Заполнение!C40)</f>
         <v/>
       </c>
-      <c r="C38" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D38" s="60"/>
+      <c r="C38" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D38" s="62"/>
       <c r="E38" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3294,11 +3292,11 @@
         <f>IF(Заполнение!C41="","",Заполнение!C41)</f>
         <v/>
       </c>
-      <c r="C39" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D39" s="60"/>
+      <c r="C39" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D39" s="62"/>
       <c r="E39" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3321,11 +3319,11 @@
         <f>IF(Заполнение!C42="","",Заполнение!C42)</f>
         <v/>
       </c>
-      <c r="C40" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D40" s="60"/>
+      <c r="C40" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D40" s="62"/>
       <c r="E40" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3348,11 +3346,11 @@
         <f>IF(Заполнение!C43="","",Заполнение!C43)</f>
         <v/>
       </c>
-      <c r="C41" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D41" s="60"/>
+      <c r="C41" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D41" s="62"/>
       <c r="E41" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3375,11 +3373,11 @@
         <f>IF(Заполнение!C44="","",Заполнение!C44)</f>
         <v/>
       </c>
-      <c r="C42" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D42" s="60"/>
+      <c r="C42" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D42" s="62"/>
       <c r="E42" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3402,11 +3400,11 @@
         <f>IF(Заполнение!C45="","",Заполнение!C45)</f>
         <v/>
       </c>
-      <c r="C43" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D43" s="60"/>
+      <c r="C43" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D43" s="62"/>
       <c r="E43" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3429,11 +3427,11 @@
         <f>IF(Заполнение!C46="","",Заполнение!C46)</f>
         <v/>
       </c>
-      <c r="C44" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D44" s="60"/>
+      <c r="C44" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D44" s="62"/>
       <c r="E44" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3456,11 +3454,11 @@
         <f>IF(Заполнение!C47="","",Заполнение!C47)</f>
         <v/>
       </c>
-      <c r="C45" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D45" s="60"/>
+      <c r="C45" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D45" s="62"/>
       <c r="E45" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3483,11 +3481,11 @@
         <f>IF(Заполнение!C48="","",Заполнение!C48)</f>
         <v/>
       </c>
-      <c r="C46" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D46" s="60"/>
+      <c r="C46" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D46" s="62"/>
       <c r="E46" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3510,11 +3508,11 @@
         <f>IF(Заполнение!C49="","",Заполнение!C49)</f>
         <v/>
       </c>
-      <c r="C47" s="59" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D47" s="60"/>
+      <c r="C47" s="61" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D47" s="62"/>
       <c r="E47" s="25" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3537,11 +3535,11 @@
         <f>IF(Заполнение!C50="","",Заполнение!C50)</f>
         <v/>
       </c>
-      <c r="C48" s="61" t="e">
-        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D48" s="62"/>
+      <c r="C48" s="68" t="e">
+        <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D48" s="69"/>
       <c r="E48" s="29" t="e">
         <f>IF(Заполнение!#REF!="","",Заполнение!#REF!)</f>
         <v>#REF!</v>
@@ -3556,307 +3554,307 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C49" s="57"/>
-      <c r="D49" s="57"/>
+      <c r="C49" s="67"/>
+      <c r="D49" s="67"/>
       <c r="G49" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="65" t="s">
+      <c r="A51" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="65"/>
-      <c r="C51" s="65"/>
-      <c r="D51" s="65"/>
-      <c r="E51" s="65"/>
-      <c r="F51" s="66" t="s">
+      <c r="B51" s="59"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="G51" s="66"/>
+      <c r="G51" s="60"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="65"/>
-      <c r="B52" s="65"/>
-      <c r="C52" s="65"/>
-      <c r="D52" s="65"/>
-      <c r="E52" s="65"/>
-      <c r="F52" s="66" t="s">
+      <c r="A52" s="59"/>
+      <c r="B52" s="59"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="59"/>
+      <c r="F52" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="G52" s="66"/>
+      <c r="G52" s="60"/>
     </row>
     <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="65" t="s">
+      <c r="A53" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="65"/>
-      <c r="C53" s="65"/>
-      <c r="D53" s="65"/>
-      <c r="E53" s="65"/>
-      <c r="F53" s="66" t="str">
+      <c r="B53" s="59"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="60" t="str">
         <f ca="1">"Дата: " &amp; TEXT(TODAY(),"ДД.ММ.ГГГГ")</f>
-        <v>Дата: 23.03.2023</v>
-      </c>
-      <c r="G53" s="66"/>
+        <v>Дата: 25.03.2023</v>
+      </c>
+      <c r="G53" s="60"/>
       <c r="I53" s="35"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="57"/>
-      <c r="D54" s="57"/>
+      <c r="C54" s="67"/>
+      <c r="D54" s="67"/>
       <c r="G54" s="13"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
+      <c r="C55" s="67"/>
+      <c r="D55" s="67"/>
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C56" s="57"/>
-      <c r="D56" s="57"/>
+      <c r="C56" s="67"/>
+      <c r="D56" s="67"/>
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="57"/>
-      <c r="D57" s="57"/>
+      <c r="C57" s="67"/>
+      <c r="D57" s="67"/>
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C58" s="57"/>
-      <c r="D58" s="57"/>
+      <c r="C58" s="67"/>
+      <c r="D58" s="67"/>
       <c r="G58" s="13"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="57"/>
-      <c r="D62" s="57"/>
+      <c r="C62" s="67"/>
+      <c r="D62" s="67"/>
       <c r="G62" s="13"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C63" s="57"/>
-      <c r="D63" s="57"/>
+      <c r="C63" s="67"/>
+      <c r="D63" s="67"/>
       <c r="G63" s="13"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C64" s="57"/>
-      <c r="D64" s="57"/>
+      <c r="C64" s="67"/>
+      <c r="D64" s="67"/>
       <c r="G64" s="13"/>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="57"/>
-      <c r="D65" s="57"/>
+      <c r="C65" s="67"/>
+      <c r="D65" s="67"/>
       <c r="G65" s="13"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="57"/>
-      <c r="D66" s="57"/>
+      <c r="C66" s="67"/>
+      <c r="D66" s="67"/>
       <c r="G66" s="13"/>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="57"/>
-      <c r="D67" s="57"/>
+      <c r="C67" s="67"/>
+      <c r="D67" s="67"/>
       <c r="G67" s="13"/>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="57"/>
-      <c r="D68" s="57"/>
+      <c r="C68" s="67"/>
+      <c r="D68" s="67"/>
       <c r="G68" s="13"/>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="57"/>
-      <c r="D69" s="57"/>
+      <c r="C69" s="67"/>
+      <c r="D69" s="67"/>
       <c r="G69" s="13"/>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="57"/>
-      <c r="D70" s="57"/>
+      <c r="C70" s="67"/>
+      <c r="D70" s="67"/>
       <c r="G70" s="13"/>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="57"/>
-      <c r="D71" s="57"/>
+      <c r="C71" s="67"/>
+      <c r="D71" s="67"/>
       <c r="G71" s="13"/>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="57"/>
-      <c r="D72" s="57"/>
+      <c r="C72" s="67"/>
+      <c r="D72" s="67"/>
       <c r="G72" s="13"/>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="57"/>
-      <c r="D73" s="57"/>
+      <c r="C73" s="67"/>
+      <c r="D73" s="67"/>
       <c r="G73" s="13"/>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="57"/>
-      <c r="D74" s="57"/>
+      <c r="C74" s="67"/>
+      <c r="D74" s="67"/>
       <c r="G74" s="13"/>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="57"/>
-      <c r="D75" s="57"/>
+      <c r="C75" s="67"/>
+      <c r="D75" s="67"/>
       <c r="G75" s="13"/>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="57"/>
-      <c r="D76" s="57"/>
+      <c r="C76" s="67"/>
+      <c r="D76" s="67"/>
       <c r="G76" s="13"/>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C77" s="57"/>
-      <c r="D77" s="57"/>
+      <c r="C77" s="67"/>
+      <c r="D77" s="67"/>
       <c r="G77" s="13"/>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C78" s="57"/>
-      <c r="D78" s="57"/>
+      <c r="C78" s="67"/>
+      <c r="D78" s="67"/>
       <c r="G78" s="13"/>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="57"/>
-      <c r="D79" s="57"/>
+      <c r="C79" s="67"/>
+      <c r="D79" s="67"/>
       <c r="G79" s="13"/>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C80" s="57"/>
-      <c r="D80" s="57"/>
+      <c r="C80" s="67"/>
+      <c r="D80" s="67"/>
       <c r="G80" s="13"/>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C81" s="57"/>
-      <c r="D81" s="57"/>
+      <c r="C81" s="67"/>
+      <c r="D81" s="67"/>
       <c r="G81" s="13"/>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C82" s="57"/>
-      <c r="D82" s="57"/>
+      <c r="C82" s="67"/>
+      <c r="D82" s="67"/>
       <c r="G82" s="13"/>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C83" s="57"/>
-      <c r="D83" s="57"/>
+      <c r="C83" s="67"/>
+      <c r="D83" s="67"/>
       <c r="G83" s="13"/>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C84" s="57"/>
-      <c r="D84" s="57"/>
+      <c r="C84" s="67"/>
+      <c r="D84" s="67"/>
       <c r="G84" s="13"/>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C85" s="57"/>
-      <c r="D85" s="57"/>
+      <c r="C85" s="67"/>
+      <c r="D85" s="67"/>
       <c r="G85" s="13"/>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="57"/>
-      <c r="D86" s="57"/>
+      <c r="C86" s="67"/>
+      <c r="D86" s="67"/>
       <c r="G86" s="13"/>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C87" s="57"/>
-      <c r="D87" s="57"/>
+      <c r="C87" s="67"/>
+      <c r="D87" s="67"/>
       <c r="G87" s="13"/>
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C88" s="57"/>
-      <c r="D88" s="57"/>
+      <c r="C88" s="67"/>
+      <c r="D88" s="67"/>
       <c r="G88" s="13"/>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="57"/>
-      <c r="D89" s="57"/>
+      <c r="C89" s="67"/>
+      <c r="D89" s="67"/>
       <c r="G89" s="13"/>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="57"/>
-      <c r="D90" s="57"/>
+      <c r="C90" s="67"/>
+      <c r="D90" s="67"/>
       <c r="G90" s="13"/>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="57"/>
-      <c r="D91" s="57"/>
+      <c r="C91" s="67"/>
+      <c r="D91" s="67"/>
       <c r="G91" s="13"/>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="57"/>
-      <c r="D92" s="57"/>
+      <c r="C92" s="67"/>
+      <c r="D92" s="67"/>
       <c r="G92" s="13"/>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C93" s="57"/>
-      <c r="D93" s="57"/>
+      <c r="C93" s="67"/>
+      <c r="D93" s="67"/>
       <c r="G93" s="13"/>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C94" s="57"/>
-      <c r="D94" s="57"/>
+      <c r="C94" s="67"/>
+      <c r="D94" s="67"/>
       <c r="G94" s="13"/>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C95" s="57"/>
-      <c r="D95" s="57"/>
+      <c r="C95" s="67"/>
+      <c r="D95" s="67"/>
       <c r="G95" s="13"/>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C96" s="57"/>
-      <c r="D96" s="57"/>
+      <c r="C96" s="67"/>
+      <c r="D96" s="67"/>
       <c r="G96" s="13"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C97" s="57"/>
-      <c r="D97" s="57"/>
+      <c r="C97" s="67"/>
+      <c r="D97" s="67"/>
       <c r="G97" s="13"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C98" s="57"/>
-      <c r="D98" s="57"/>
+      <c r="C98" s="67"/>
+      <c r="D98" s="67"/>
       <c r="G98" s="13"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C99" s="57"/>
-      <c r="D99" s="57"/>
+      <c r="C99" s="67"/>
+      <c r="D99" s="67"/>
       <c r="G99" s="13"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C100" s="57"/>
-      <c r="D100" s="57"/>
+      <c r="C100" s="67"/>
+      <c r="D100" s="67"/>
       <c r="G100" s="13"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C101" s="57"/>
-      <c r="D101" s="57"/>
+      <c r="C101" s="67"/>
+      <c r="D101" s="67"/>
       <c r="G101" s="13"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C102" s="57"/>
-      <c r="D102" s="57"/>
+      <c r="C102" s="67"/>
+      <c r="D102" s="67"/>
       <c r="G102" s="13"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C103" s="57"/>
-      <c r="D103" s="57"/>
+      <c r="C103" s="67"/>
+      <c r="D103" s="67"/>
       <c r="G103" s="13"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C104" s="57"/>
-      <c r="D104" s="57"/>
+      <c r="C104" s="67"/>
+      <c r="D104" s="67"/>
       <c r="G104" s="13"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C105" s="57"/>
-      <c r="D105" s="57"/>
+      <c r="C105" s="67"/>
+      <c r="D105" s="67"/>
       <c r="G105" s="13"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C106" s="57"/>
-      <c r="D106" s="57"/>
+      <c r="C106" s="67"/>
+      <c r="D106" s="67"/>
       <c r="G106" s="13"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C107" s="57"/>
-      <c r="D107" s="57"/>
+      <c r="C107" s="67"/>
+      <c r="D107" s="67"/>
       <c r="G107" s="13"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C108" s="57"/>
-      <c r="D108" s="57"/>
+      <c r="C108" s="67"/>
+      <c r="D108" s="67"/>
       <c r="G108" s="13"/>
     </row>
     <row r="110" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3872,6 +3870,83 @@
     </row>
   </sheetData>
   <mergeCells count="101">
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="A1:G3"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="A53:E53"/>
@@ -3896,83 +3971,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="A1:G3"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C82:D82"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0" header="0" footer="0"/>

</xml_diff>